<commit_message>
added columns to timesheet
</commit_message>
<xml_diff>
--- a/test/timesheet.xlsx
+++ b/test/timesheet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -15,9 +15,35 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>stop</t>
+  </si>
+  <si>
+    <t>interrupt</t>
+  </si>
+  <si>
+    <t>delta (time-interrupt)</t>
+  </si>
+  <si>
+    <t>activity</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,6 +80,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -343,36 +374,66 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
created monogame project for the game
</commit_message>
<xml_diff>
--- a/test/timesheet.xlsx
+++ b/test/timesheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>date</t>
   </si>
@@ -37,6 +37,21 @@
   </si>
   <si>
     <t>comments</t>
+  </si>
+  <si>
+    <t>Research/Setup</t>
+  </si>
+  <si>
+    <t>Installed Monogame and created a project for the game</t>
+  </si>
+  <si>
+    <t>11 minutes</t>
+  </si>
+  <si>
+    <t>35 minutes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Went through monogame documentation/tutorial </t>
   </si>
 </sst>
 </file>
@@ -72,8 +87,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,16 +392,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="51.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -408,6 +427,52 @@
       </c>
       <c r="G1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>43857</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.27291666666666664</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.15555555555555556</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>43863</v>
+      </c>
+      <c r="B3" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.1076388888888889</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added enemy ghost and player sprites, implemented some enemy logic, updated timesheet
</commit_message>
<xml_diff>
--- a/test/timesheet.xlsx
+++ b/test/timesheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>date</t>
   </si>
@@ -52,6 +52,24 @@
   </si>
   <si>
     <t xml:space="preserve">Went through monogame documentation/tutorial </t>
+  </si>
+  <si>
+    <t>4 hours 30 minutes</t>
+  </si>
+  <si>
+    <t>Research/Programming</t>
+  </si>
+  <si>
+    <t>Set up enemy class with enemy ghost that follows player</t>
+  </si>
+  <si>
+    <t>Created sprite for protagonist and created animation classes</t>
+  </si>
+  <si>
+    <t>2 hours 30 minutes</t>
+  </si>
+  <si>
+    <t>Tried and failed to set up monogame extended third party library</t>
   </si>
 </sst>
 </file>
@@ -392,18 +410,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="51.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="59.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -434,10 +453,10 @@
         <v>43857</v>
       </c>
       <c r="B2" s="2">
-        <v>0.27291666666666664</v>
+        <v>0.7729166666666667</v>
       </c>
       <c r="C2" s="2">
-        <v>0.15555555555555556</v>
+        <v>0.78055555555555556</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -457,10 +476,10 @@
         <v>43863</v>
       </c>
       <c r="B3" s="2">
-        <v>8.3333333333333329E-2</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="C3" s="2">
-        <v>0.1076388888888889</v>
+        <v>0.60763888888888895</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -473,6 +492,75 @@
       </c>
       <c r="G3" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>43868</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D4" s="2">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>43877</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D5" s="2">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>43884</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D6" s="2">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created new solution to work out issues with Monogame Extended
</commit_message>
<xml_diff>
--- a/test/timesheet.xlsx
+++ b/test/timesheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>date</t>
   </si>
@@ -70,6 +70,27 @@
   </si>
   <si>
     <t>Tried and failed to set up monogame extended third party library</t>
+  </si>
+  <si>
+    <t>Programming</t>
+  </si>
+  <si>
+    <t>Added code for collision detection and created attack animation for player</t>
+  </si>
+  <si>
+    <t>3 hours</t>
+  </si>
+  <si>
+    <t>Proogramming</t>
+  </si>
+  <si>
+    <t>Added hit detection and reactions for the player's attacks</t>
+  </si>
+  <si>
+    <t>3 hours 30 minutes</t>
+  </si>
+  <si>
+    <t>Created tilemap for starting room and attempted unsuccessfully to get monogame extended library working</t>
   </si>
 </sst>
 </file>
@@ -105,10 +126,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,19 +432,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="59.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="99.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -561,6 +584,75 @@
       </c>
       <c r="G6" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>43898</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>43902</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>43905</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>